<commit_message>
Python File creator v1.0 added
</commit_message>
<xml_diff>
--- a/Manuals/Review sheet template.xlsx
+++ b/Manuals/Review sheet template.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simon\Documents\Work\Programming\Ada\ADLAS Other\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simon\Documents\Work\Programming\Ada\System Checks\Manuals\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>

</xml_diff>